<commit_message>
Release NPFS to TI
</commit_message>
<xml_diff>
--- a/ITI/NPFS/CodeSystem-NPFSclasscode.xlsx
+++ b/ITI/NPFS/CodeSystem-NPFSclasscode.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>2.2.0-comment</t>
+    <t>2.2.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-08-02T08:51:52-05:00</t>
+    <t>2023-11-16T16:11:53-06:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>